<commit_message>
Cập nhật lịch dự án
</commit_message>
<xml_diff>
--- a/01. Document/DropOut_project v2011.08.25.xlsx
+++ b/01. Document/DropOut_project v2011.08.25.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Convension" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan!$A$8:$BQ$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan!$A$8:$BQ$72</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="102">
   <si>
     <t>STT</t>
   </si>
@@ -281,9 +281,6 @@
     <t>- Tham số luyện mạng</t>
   </si>
   <si>
-    <t>- Hiển thị dữ liệu từ file text</t>
-  </si>
-  <si>
     <t>- Truy vấn kết quả</t>
   </si>
   <si>
@@ -309,6 +306,24 @@
   </si>
   <si>
     <t xml:space="preserve">          - Chuẩn hóa dạng -1-&gt;1</t>
+  </si>
+  <si>
+    <t>Giao diện</t>
+  </si>
+  <si>
+    <t>Module chương trình</t>
+  </si>
+  <si>
+    <t>- Hiển thị dữ liệu từ file text, csv</t>
+  </si>
+  <si>
+    <t>- Làm sạch dữ liệu, khử nhiễu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          - Rời rạc hóa dữ liệu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- </t>
   </si>
 </sst>
 </file>
@@ -519,7 +534,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
@@ -541,6 +556,48 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF0000CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF0000CC"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0000"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0000CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -882,13 +939,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BQ69"/>
+  <dimension ref="A1:BQ72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="8" topLeftCell="H28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="8" topLeftCell="H32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomRight" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -932,7 +989,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="17">
-        <f>SUMIF($D$9:$D$65,C2,$E$9:$E$65)</f>
+        <f>SUMIF($D$9:$D$68,C2,$E$9:$E$68)</f>
         <v>0</v>
       </c>
       <c r="E2" s="11" t="s">
@@ -961,7 +1018,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="17">
-        <f>SUMIF($D$9:$D$65,#REF!,$E$9:$E$65)</f>
+        <f>SUMIF($D$9:$D$68,#REF!,$E$9:$E$68)</f>
         <v>0</v>
       </c>
       <c r="E3" s="11" t="s">
@@ -977,7 +1034,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="17">
-        <f>SUMIF($D$9:$D$65,C3,$E$9:$E$65)</f>
+        <f>SUMIF($D$9:$D$68,C3,$E$9:$E$68)</f>
         <v>0</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -988,7 +1045,7 @@
     <row r="5" spans="1:69">
       <c r="C5" s="24"/>
       <c r="D5" s="17">
-        <f>SUMIF($D$9:$D$65,C5,$E$9:$E$65)</f>
+        <f>SUMIF($D$9:$D$68,C5,$E$9:$E$68)</f>
         <v>0</v>
       </c>
       <c r="E5" s="11"/>
@@ -997,7 +1054,7 @@
     <row r="6" spans="1:69">
       <c r="C6" s="24"/>
       <c r="D6" s="17">
-        <f>SUMIF($D$9:$D$65,C6,$E$9:$E$65)</f>
+        <f>SUMIF($D$9:$D$68,C6,$E$9:$E$68)</f>
         <v>0</v>
       </c>
       <c r="E6" s="11"/>
@@ -1526,11 +1583,11 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="4">
-        <f>IFERROR( HLOOKUP("BE",J10:BD$69,$A$69-$A10+1,FALSE),0)+ IFERROR( HLOOKUP("B",J10:BD$69,$A$69-$A10+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J10:BD$72,$A$72-$A10+1,FALSE),0)+ IFERROR( HLOOKUP("B",J10:BD$72,$A$72-$A10+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G10" s="4">
-        <f>IFERROR( HLOOKUP("BE",J10:BD$69,$A$69-$A10+1,FALSE),0)+ IFERROR( HLOOKUP("E",J10:BD$69,$A$69-$A10+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J10:BD$72,$A$72-$A10+1,FALSE),0)+ IFERROR( HLOOKUP("E",J10:BD$72,$A$72-$A10+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H10" s="4" t="s">
@@ -1617,11 +1674,11 @@
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="4">
-        <f>IFERROR( HLOOKUP("BE",J11:BD$69,$A$69-$A11+1,FALSE),0)+ IFERROR( HLOOKUP("B",J11:BD$69,$A$69-$A11+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J11:BD$72,$A$72-$A11+1,FALSE),0)+ IFERROR( HLOOKUP("B",J11:BD$72,$A$72-$A11+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G11" s="4">
-        <f>IFERROR( HLOOKUP("BE",J11:BD$69,$A$69-$A11+1,FALSE),0)+ IFERROR( HLOOKUP("E",J11:BD$69,$A$69-$A11+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J11:BD$72,$A$72-$A11+1,FALSE),0)+ IFERROR( HLOOKUP("E",J11:BD$72,$A$72-$A11+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H11" s="4" t="s">
@@ -1779,11 +1836,11 @@
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="13">
-        <f>IFERROR( HLOOKUP("BE",J13:BD$69,$A$69-$A13+1,FALSE),0)+ IFERROR( HLOOKUP("B",J13:BD$69,$A$69-$A13+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J13:BD$72,$A$72-$A13+1,FALSE),0)+ IFERROR( HLOOKUP("B",J13:BD$72,$A$72-$A13+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G13" s="13">
-        <f>IFERROR( HLOOKUP("BE",J13:BD$69,$A$69-$A13+1,FALSE),0)+ IFERROR( HLOOKUP("E",J13:BD$69,$A$69-$A13+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J13:BD$72,$A$72-$A13+1,FALSE),0)+ IFERROR( HLOOKUP("E",J13:BD$72,$A$72-$A13+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H13" s="4" t="s">
@@ -1943,11 +2000,11 @@
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="4">
-        <f>IFERROR( HLOOKUP("BE",J15:BD$69,$A$69-$A15+1,FALSE),0)+ IFERROR( HLOOKUP("B",J15:BD$69,$A$69-$A15+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J15:BD$72,$A$72-$A15+1,FALSE),0)+ IFERROR( HLOOKUP("B",J15:BD$72,$A$72-$A15+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G15" s="4">
-        <f>IFERROR( HLOOKUP("BE",J15:BD$69,$A$69-$A15+1,FALSE),0)+ IFERROR( HLOOKUP("E",J15:BD$69,$A$69-$A15+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J15:BD$72,$A$72-$A15+1,FALSE),0)+ IFERROR( HLOOKUP("E",J15:BD$72,$A$72-$A15+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H15" s="4" t="s">
@@ -2044,11 +2101,11 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="4">
-        <f>IFERROR( HLOOKUP("BE",J16:BD$69,$A$69-$A16+1,FALSE),0)+ IFERROR( HLOOKUP("B",J16:BD$69,$A$69-$A16+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J16:BD$72,$A$72-$A16+1,FALSE),0)+ IFERROR( HLOOKUP("B",J16:BD$72,$A$72-$A16+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G16" s="4">
-        <f>IFERROR( HLOOKUP("BE",J16:BD$69,$A$69-$A16+1,FALSE),0)+ IFERROR( HLOOKUP("E",J16:BD$69,$A$69-$A16+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J16:BD$72,$A$72-$A16+1,FALSE),0)+ IFERROR( HLOOKUP("E",J16:BD$72,$A$72-$A16+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H16" s="4" t="s">
@@ -2228,11 +2285,11 @@
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="4">
-        <f>IFERROR( HLOOKUP("BE",J18:BD$69,$A$69-$A18+1,FALSE),0)+ IFERROR( HLOOKUP("B",J18:BD$69,$A$69-$A18+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J18:BD$72,$A$72-$A18+1,FALSE),0)+ IFERROR( HLOOKUP("B",J18:BD$72,$A$72-$A18+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G18" s="4">
-        <f>IFERROR( HLOOKUP("BE",J18:BD$69,$A$69-$A18+1,FALSE),0)+ IFERROR( HLOOKUP("E",J18:BD$69,$A$69-$A18+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J18:BD$72,$A$72-$A18+1,FALSE),0)+ IFERROR( HLOOKUP("E",J18:BD$72,$A$72-$A18+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H18" s="4" t="s">
@@ -2319,11 +2376,11 @@
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="4">
-        <f>IFERROR( HLOOKUP("BE",J19:BD$69,$A$69-$A19+1,FALSE),0)+ IFERROR( HLOOKUP("B",J19:BD$69,$A$69-$A19+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J19:BD$72,$A$72-$A19+1,FALSE),0)+ IFERROR( HLOOKUP("B",J19:BD$72,$A$72-$A19+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G19" s="4">
-        <f>IFERROR( HLOOKUP("BE",J19:BD$69,$A$69-$A19+1,FALSE),0)+ IFERROR( HLOOKUP("E",J19:BD$69,$A$69-$A19+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J19:BD$72,$A$72-$A19+1,FALSE),0)+ IFERROR( HLOOKUP("E",J19:BD$72,$A$72-$A19+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H19" s="4" t="s">
@@ -2414,11 +2471,11 @@
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="4">
-        <f>IFERROR( HLOOKUP("BE",J20:BD$69,$A$69-$A20+1,FALSE),0)+ IFERROR( HLOOKUP("B",J20:BD$69,$A$69-$A20+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J20:BD$72,$A$72-$A20+1,FALSE),0)+ IFERROR( HLOOKUP("B",J20:BD$72,$A$72-$A20+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G20" s="4">
-        <f>IFERROR( HLOOKUP("BE",J20:BD$69,$A$69-$A20+1,FALSE),0)+ IFERROR( HLOOKUP("E",J20:BD$69,$A$69-$A20+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J20:BD$72,$A$72-$A20+1,FALSE),0)+ IFERROR( HLOOKUP("E",J20:BD$72,$A$72-$A20+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H20" s="4" t="s">
@@ -2509,11 +2566,11 @@
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="4">
-        <f>IFERROR( HLOOKUP("BE",J21:BD$69,$A$69-$A21+1,FALSE),0)+ IFERROR( HLOOKUP("B",J21:BD$69,$A$69-$A21+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J21:BD$72,$A$72-$A21+1,FALSE),0)+ IFERROR( HLOOKUP("B",J21:BD$72,$A$72-$A21+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G21" s="4">
-        <f>IFERROR( HLOOKUP("BE",J21:BD$69,$A$69-$A21+1,FALSE),0)+ IFERROR( HLOOKUP("E",J21:BD$69,$A$69-$A21+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J21:BD$72,$A$72-$A21+1,FALSE),0)+ IFERROR( HLOOKUP("E",J21:BD$72,$A$72-$A21+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H21" s="4" t="s">
@@ -2600,11 +2657,11 @@
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="4">
-        <f>IFERROR( HLOOKUP("BE",J22:BD$69,$A$69-$A22+1,FALSE),0)+ IFERROR( HLOOKUP("B",J22:BD$69,$A$69-$A22+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J22:BD$72,$A$72-$A22+1,FALSE),0)+ IFERROR( HLOOKUP("B",J22:BD$72,$A$72-$A22+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G22" s="4">
-        <f>IFERROR( HLOOKUP("BE",J22:BD$69,$A$69-$A22+1,FALSE),0)+ IFERROR( HLOOKUP("E",J22:BD$69,$A$69-$A22+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J22:BD$72,$A$72-$A22+1,FALSE),0)+ IFERROR( HLOOKUP("E",J22:BD$72,$A$72-$A22+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H22" s="4"/>
@@ -2762,11 +2819,11 @@
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="4">
-        <f>IFERROR( HLOOKUP("BE",J24:BD$69,$A$69-$A24+1,FALSE),0)+ IFERROR( HLOOKUP("B",J24:BD$69,$A$69-$A24+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J24:BD$72,$A$72-$A24+1,FALSE),0)+ IFERROR( HLOOKUP("B",J24:BD$72,$A$72-$A24+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G24" s="4">
-        <f>IFERROR( HLOOKUP("BE",J24:BD$69,$A$69-$A24+1,FALSE),0)+ IFERROR( HLOOKUP("E",J24:BD$69,$A$69-$A24+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J24:BD$72,$A$72-$A24+1,FALSE),0)+ IFERROR( HLOOKUP("E",J24:BD$72,$A$72-$A24+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H24" s="4" t="s">
@@ -2853,11 +2910,11 @@
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="4">
-        <f>IFERROR( HLOOKUP("BE",J25:BD$69,$A$69-$A25+1,FALSE),0)+ IFERROR( HLOOKUP("B",J25:BD$69,$A$69-$A25+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J25:BD$72,$A$72-$A25+1,FALSE),0)+ IFERROR( HLOOKUP("B",J25:BD$72,$A$72-$A25+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G25" s="4">
-        <f>IFERROR( HLOOKUP("BE",J25:BD$69,$A$69-$A25+1,FALSE),0)+ IFERROR( HLOOKUP("E",J25:BD$69,$A$69-$A25+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J25:BD$72,$A$72-$A25+1,FALSE),0)+ IFERROR( HLOOKUP("E",J25:BD$72,$A$72-$A25+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H25" s="4" t="s">
@@ -2944,11 +3001,11 @@
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="4">
-        <f>IFERROR( HLOOKUP("BE",J26:BD$69,$A$69-$A26+1,FALSE),0)+ IFERROR( HLOOKUP("B",J26:BD$69,$A$69-$A26+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J26:BD$72,$A$72-$A26+1,FALSE),0)+ IFERROR( HLOOKUP("B",J26:BD$72,$A$72-$A26+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G26" s="4">
-        <f>IFERROR( HLOOKUP("BE",J26:BD$69,$A$69-$A26+1,FALSE),0)+ IFERROR( HLOOKUP("E",J26:BD$69,$A$69-$A26+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J26:BD$72,$A$72-$A26+1,FALSE),0)+ IFERROR( HLOOKUP("E",J26:BD$72,$A$72-$A26+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H26" s="4" t="s">
@@ -3035,11 +3092,11 @@
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="4">
-        <f>IFERROR( HLOOKUP("BE",J27:BD$69,$A$69-$A27+1,FALSE),0)+ IFERROR( HLOOKUP("B",J27:BD$69,$A$69-$A27+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J27:BD$72,$A$72-$A27+1,FALSE),0)+ IFERROR( HLOOKUP("B",J27:BD$72,$A$72-$A27+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G27" s="4">
-        <f>IFERROR( HLOOKUP("BE",J27:BD$69,$A$69-$A27+1,FALSE),0)+ IFERROR( HLOOKUP("E",J27:BD$69,$A$69-$A27+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J27:BD$72,$A$72-$A27+1,FALSE),0)+ IFERROR( HLOOKUP("E",J27:BD$72,$A$72-$A27+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H27" s="4" t="s">
@@ -3128,11 +3185,11 @@
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="4">
-        <f>IFERROR( HLOOKUP("BE",J28:BD$69,$A$69-$A28+1,FALSE),0)+ IFERROR( HLOOKUP("B",J28:BD$69,$A$69-$A28+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J28:BD$72,$A$72-$A28+1,FALSE),0)+ IFERROR( HLOOKUP("B",J28:BD$72,$A$72-$A28+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G28" s="4">
-        <f>IFERROR( HLOOKUP("BE",J28:BD$69,$A$69-$A28+1,FALSE),0)+ IFERROR( HLOOKUP("E",J28:BD$69,$A$69-$A28+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J28:BD$72,$A$72-$A28+1,FALSE),0)+ IFERROR( HLOOKUP("E",J28:BD$72,$A$72-$A28+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H28" s="4" t="s">
@@ -3217,11 +3274,11 @@
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="4">
-        <f>IFERROR( HLOOKUP("BE",J29:BD$69,$A$69-$A29+1,FALSE),0)+ IFERROR( HLOOKUP("B",J29:BD$69,$A$69-$A29+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J29:BD$72,$A$72-$A29+1,FALSE),0)+ IFERROR( HLOOKUP("B",J29:BD$72,$A$72-$A29+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G29" s="4">
-        <f>IFERROR( HLOOKUP("BE",J29:BD$69,$A$69-$A29+1,FALSE),0)+ IFERROR( HLOOKUP("E",J29:BD$69,$A$69-$A29+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J29:BD$72,$A$72-$A29+1,FALSE),0)+ IFERROR( HLOOKUP("E",J29:BD$72,$A$72-$A29+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H29" s="4" t="s">
@@ -3314,11 +3371,11 @@
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="4">
-        <f>IFERROR( HLOOKUP("BE",J30:BD$69,$A$69-$A30+1,FALSE),0)+ IFERROR( HLOOKUP("B",J30:BD$69,$A$69-$A30+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J30:BD$72,$A$72-$A30+1,FALSE),0)+ IFERROR( HLOOKUP("B",J30:BD$72,$A$72-$A30+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G30" s="4">
-        <f>IFERROR( HLOOKUP("BE",J30:BD$69,$A$69-$A30+1,FALSE),0)+ IFERROR( HLOOKUP("E",J30:BD$69,$A$69-$A30+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J30:BD$72,$A$72-$A30+1,FALSE),0)+ IFERROR( HLOOKUP("E",J30:BD$72,$A$72-$A30+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H30" s="4" t="s">
@@ -3482,11 +3539,11 @@
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="4">
-        <f>IFERROR( HLOOKUP("BE",J32:BD$69,$A$69-$A32+1,FALSE),0)+ IFERROR( HLOOKUP("B",J32:BD$69,$A$69-$A32+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J32:BD$72,$A$72-$A32+1,FALSE),0)+ IFERROR( HLOOKUP("B",J32:BD$72,$A$72-$A32+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G32" s="4">
-        <f>IFERROR( HLOOKUP("BE",J32:BD$69,$A$69-$A32+1,FALSE),0)+ IFERROR( HLOOKUP("E",J32:BD$69,$A$69-$A32+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J32:BD$72,$A$72-$A32+1,FALSE),0)+ IFERROR( HLOOKUP("E",J32:BD$72,$A$72-$A32+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H32" s="4" t="s">
@@ -3571,11 +3628,11 @@
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="4">
-        <f>IFERROR( HLOOKUP("BE",J33:BD$69,$A$69-$A33+1,FALSE),0)+ IFERROR( HLOOKUP("B",J33:BD$69,$A$69-$A33+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J33:BD$72,$A$72-$A33+1,FALSE),0)+ IFERROR( HLOOKUP("B",J33:BD$72,$A$72-$A33+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G33" s="4">
-        <f>IFERROR( HLOOKUP("BE",J33:BD$69,$A$69-$A33+1,FALSE),0)+ IFERROR( HLOOKUP("E",J33:BD$69,$A$69-$A33+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J33:BD$72,$A$72-$A33+1,FALSE),0)+ IFERROR( HLOOKUP("E",J33:BD$72,$A$72-$A33+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H33" s="4" t="s">
@@ -3664,11 +3721,11 @@
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="4">
-        <f>IFERROR( HLOOKUP("BE",J34:BD$69,$A$69-$A34+1,FALSE),0)+ IFERROR( HLOOKUP("B",J34:BD$69,$A$69-$A34+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J34:BD$72,$A$72-$A34+1,FALSE),0)+ IFERROR( HLOOKUP("B",J34:BD$72,$A$72-$A34+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G34" s="4">
-        <f>IFERROR( HLOOKUP("BE",J34:BD$69,$A$69-$A34+1,FALSE),0)+ IFERROR( HLOOKUP("E",J34:BD$69,$A$69-$A34+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J34:BD$72,$A$72-$A34+1,FALSE),0)+ IFERROR( HLOOKUP("E",J34:BD$72,$A$72-$A34+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H34" s="4" t="s">
@@ -3765,11 +3822,11 @@
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="4">
-        <f>IFERROR( HLOOKUP("BE",J35:BD$69,$A$69-$A35+1,FALSE),0)+ IFERROR( HLOOKUP("B",J35:BD$69,$A$69-$A35+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J35:BD$72,$A$72-$A35+1,FALSE),0)+ IFERROR( HLOOKUP("B",J35:BD$72,$A$72-$A35+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G35" s="4">
-        <f>IFERROR( HLOOKUP("BE",J35:BD$69,$A$69-$A35+1,FALSE),0)+ IFERROR( HLOOKUP("E",J35:BD$69,$A$69-$A35+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J35:BD$72,$A$72-$A35+1,FALSE),0)+ IFERROR( HLOOKUP("E",J35:BD$72,$A$72-$A35+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H35" s="4" t="s">
@@ -3860,11 +3917,11 @@
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="4">
-        <f>IFERROR( HLOOKUP("BE",J36:BD$69,$A$69-$A36+1,FALSE),0)+ IFERROR( HLOOKUP("B",J36:BD$69,$A$69-$A36+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J36:BD$72,$A$72-$A36+1,FALSE),0)+ IFERROR( HLOOKUP("B",J36:BD$72,$A$72-$A36+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="G36" s="4">
-        <f>IFERROR( HLOOKUP("BE",J36:BD$69,$A$69-$A36+1,FALSE),0)+ IFERROR( HLOOKUP("E",J36:BD$69,$A$69-$A36+1,FALSE),0)</f>
+        <f>IFERROR( HLOOKUP("BE",J36:BD$72,$A$72-$A36+1,FALSE),0)+ IFERROR( HLOOKUP("E",J36:BD$72,$A$72-$A36+1,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="H36" s="4" t="s">
@@ -3946,12 +4003,18 @@
       <c r="C37" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E37" s="3"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="3"/>
+      <c r="H37" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="17"/>
@@ -3984,11 +4047,21 @@
       <c r="AM37" s="1"/>
       <c r="AN37" s="17"/>
       <c r="AO37" s="17"/>
-      <c r="AP37" s="1"/>
-      <c r="AQ37" s="1"/>
-      <c r="AR37" s="1"/>
-      <c r="AS37" s="1"/>
-      <c r="AT37" s="1"/>
+      <c r="AP37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT37" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AU37" s="17"/>
       <c r="AV37" s="17"/>
       <c r="AW37" s="1"/>
@@ -4019,7 +4092,7 @@
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -4089,9 +4162,6 @@
       <c r="BQ38" s="17"/>
     </row>
     <row r="39" spans="1:69">
-      <c r="A39">
-        <v>30</v>
-      </c>
       <c r="B39" s="3"/>
       <c r="C39" s="31"/>
       <c r="D39" s="3"/>
@@ -4167,7 +4237,7 @@
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -4242,14 +4312,20 @@
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="D41" s="3"/>
+        <v>98</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E41" s="3"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="3"/>
+      <c r="H41" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="17"/>
@@ -4314,14 +4390,20 @@
     <row r="42" spans="1:69">
       <c r="B42" s="3"/>
       <c r="C42" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="D42" s="3"/>
+        <v>99</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E42" s="3"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="3"/>
+      <c r="H42" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="17"/>
@@ -4386,14 +4468,20 @@
     <row r="43" spans="1:69">
       <c r="B43" s="3"/>
       <c r="C43" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="D43" s="3"/>
+        <v>88</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E43" s="3"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="3"/>
+      <c r="H43" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="17"/>
@@ -4457,8 +4545,8 @@
     </row>
     <row r="44" spans="1:69">
       <c r="B44" s="3"/>
-      <c r="C44" s="3" t="s">
-        <v>96</v>
+      <c r="C44" s="35" t="s">
+        <v>91</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -4529,15 +4617,21 @@
     </row>
     <row r="45" spans="1:69">
       <c r="B45" s="3"/>
-      <c r="C45" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D45" s="3"/>
+      <c r="C45" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E45" s="3"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="3"/>
+      <c r="H45" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="17"/>
@@ -4601,13 +4695,21 @@
     </row>
     <row r="46" spans="1:69">
       <c r="B46" s="3"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="3"/>
+      <c r="C46" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E46" s="3"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="3"/>
+      <c r="H46" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="17"/>
@@ -4671,13 +4773,21 @@
     </row>
     <row r="47" spans="1:69">
       <c r="B47" s="3"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="3"/>
+      <c r="C47" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E47" s="3"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="3"/>
+      <c r="H47" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="17"/>
@@ -4741,9 +4851,7 @@
     </row>
     <row r="48" spans="1:69">
       <c r="B48" s="3"/>
-      <c r="C48" s="35" t="s">
-        <v>93</v>
-      </c>
+      <c r="C48" s="36"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="4"/>
@@ -4813,9 +4921,7 @@
     </row>
     <row r="49" spans="1:69">
       <c r="B49" s="3"/>
-      <c r="C49" s="31" t="s">
-        <v>86</v>
-      </c>
+      <c r="C49" s="36"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="4"/>
@@ -4885,8 +4991,8 @@
     </row>
     <row r="50" spans="1:69">
       <c r="B50" s="3"/>
-      <c r="C50" s="31" t="s">
-        <v>88</v>
+      <c r="C50" s="35" t="s">
+        <v>92</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -4957,8 +5063,12 @@
     </row>
     <row r="51" spans="1:69">
       <c r="B51" s="3"/>
-      <c r="C51" s="33"/>
-      <c r="D51" s="3"/>
+      <c r="C51" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E51" s="3"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -5027,10 +5137,12 @@
     </row>
     <row r="52" spans="1:69">
       <c r="B52" s="3"/>
-      <c r="C52" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="D52" s="3"/>
+      <c r="C52" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E52" s="3"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
@@ -5099,7 +5211,9 @@
     </row>
     <row r="53" spans="1:69">
       <c r="B53" s="3"/>
-      <c r="C53" s="31"/>
+      <c r="C53" s="31" t="s">
+        <v>101</v>
+      </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="4"/>
@@ -5169,7 +5283,7 @@
     </row>
     <row r="54" spans="1:69">
       <c r="B54" s="3"/>
-      <c r="C54" s="34"/>
+      <c r="C54" s="33"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="4"/>
@@ -5239,7 +5353,9 @@
     </row>
     <row r="55" spans="1:69">
       <c r="B55" s="3"/>
-      <c r="C55" s="34"/>
+      <c r="C55" s="32" t="s">
+        <v>93</v>
+      </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="4"/>
@@ -5309,7 +5425,7 @@
     </row>
     <row r="56" spans="1:69">
       <c r="B56" s="3"/>
-      <c r="C56" s="34"/>
+      <c r="C56" s="31"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="4"/>
@@ -5448,11 +5564,8 @@
       <c r="BQ57" s="17"/>
     </row>
     <row r="58" spans="1:69">
-      <c r="A58">
-        <v>33</v>
-      </c>
       <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
+      <c r="C58" s="34"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="F58" s="4"/>
@@ -5521,33 +5634,14 @@
       <c r="BQ58" s="17"/>
     </row>
     <row r="59" spans="1:69">
-      <c r="A59">
-        <v>34</v>
-      </c>
-      <c r="B59" s="3">
-        <v>20</v>
-      </c>
-      <c r="C59" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="B59" s="3"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="3"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="4">
-        <f>IFERROR( HLOOKUP("BE",J59:BD$69,$A$69-$A59+1,FALSE),0)+ IFERROR( HLOOKUP("B",J59:BD$69,$A$69-$A59+1,FALSE),0)</f>
-        <v>40795</v>
-      </c>
-      <c r="G59" s="4">
-        <f>IFERROR( HLOOKUP("BE",J59:BD$69,$A$69-$A59+1,FALSE),0)+ IFERROR( HLOOKUP("E",J59:BD$69,$A$69-$A59+1,FALSE),0)</f>
-        <v>40809</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I59" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="3"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="17"/>
@@ -5563,51 +5657,21 @@
       <c r="V59" s="1"/>
       <c r="W59" s="1"/>
       <c r="X59" s="1"/>
-      <c r="Y59" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z59" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA59" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB59" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC59" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD59" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE59" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF59" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AG59" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="AH59" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="AI59" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AJ59" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AK59" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AL59" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AM59" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="Y59" s="1"/>
+      <c r="Z59" s="17"/>
+      <c r="AA59" s="17"/>
+      <c r="AB59" s="1"/>
+      <c r="AC59" s="1"/>
+      <c r="AD59" s="1"/>
+      <c r="AE59" s="1"/>
+      <c r="AF59" s="1"/>
+      <c r="AG59" s="17"/>
+      <c r="AH59" s="17"/>
+      <c r="AI59" s="1"/>
+      <c r="AJ59" s="1"/>
+      <c r="AK59" s="1"/>
+      <c r="AL59" s="1"/>
+      <c r="AM59" s="1"/>
       <c r="AN59" s="17"/>
       <c r="AO59" s="17"/>
       <c r="AP59" s="1"/>
@@ -5640,27 +5704,14 @@
       <c r="BQ59" s="17"/>
     </row>
     <row r="60" spans="1:69">
-      <c r="A60">
-        <v>35</v>
-      </c>
-      <c r="B60" s="3">
-        <v>21</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
-      <c r="H60" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="H60" s="4"/>
+      <c r="I60" s="3"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="17"/>
@@ -5724,26 +5775,16 @@
     </row>
     <row r="61" spans="1:69">
       <c r="A61">
-        <v>36</v>
-      </c>
-      <c r="B61" s="3">
-        <v>22</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
-      <c r="H61" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I61" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="H61" s="4"/>
+      <c r="I61" s="3"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="17"/>
@@ -5807,31 +5848,31 @@
     </row>
     <row r="62" spans="1:69">
       <c r="A62">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B62" s="3">
-        <v>23</v>
-      </c>
-      <c r="C62" s="27" t="s">
-        <v>35</v>
+        <v>20</v>
+      </c>
+      <c r="C62" s="23" t="s">
+        <v>34</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="4">
-        <f>IFERROR( HLOOKUP("BE",J62:BD$69,$A$69-$A62+1,FALSE),0)+ IFERROR( HLOOKUP("B",J62:BD$69,$A$69-$A62+1,FALSE),0)</f>
-        <v>40821</v>
+        <f>IFERROR( HLOOKUP("BE",J62:BD$72,$A$72-$A62+1,FALSE),0)+ IFERROR( HLOOKUP("B",J62:BD$72,$A$72-$A62+1,FALSE),0)</f>
+        <v>40795</v>
       </c>
       <c r="G62" s="4">
-        <f>IFERROR( HLOOKUP("BE",J62:BD$69,$A$69-$A62+1,FALSE),0)+ IFERROR( HLOOKUP("E",J62:BD$69,$A$69-$A62+1,FALSE),0)</f>
-        <v>40821</v>
+        <f>IFERROR( HLOOKUP("BE",J62:BD$72,$A$72-$A62+1,FALSE),0)+ IFERROR( HLOOKUP("E",J62:BD$72,$A$72-$A62+1,FALSE),0)</f>
+        <v>40809</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
@@ -5848,21 +5889,51 @@
       <c r="V62" s="1"/>
       <c r="W62" s="1"/>
       <c r="X62" s="1"/>
-      <c r="Y62" s="1"/>
-      <c r="Z62" s="17"/>
-      <c r="AA62" s="17"/>
-      <c r="AB62" s="1"/>
-      <c r="AC62" s="1"/>
-      <c r="AD62" s="1"/>
-      <c r="AE62" s="1"/>
-      <c r="AF62" s="1"/>
-      <c r="AG62" s="17"/>
-      <c r="AH62" s="17"/>
-      <c r="AI62" s="1"/>
-      <c r="AJ62" s="1"/>
-      <c r="AK62" s="1"/>
-      <c r="AL62" s="1"/>
-      <c r="AM62" s="1"/>
+      <c r="Y62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z62" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA62" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG62" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH62" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM62" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AN62" s="17"/>
       <c r="AO62" s="17"/>
       <c r="AP62" s="1"/>
@@ -5874,9 +5945,7 @@
       <c r="AV62" s="17"/>
       <c r="AW62" s="1"/>
       <c r="AX62" s="1"/>
-      <c r="AY62" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="AY62" s="1"/>
       <c r="AZ62" s="1"/>
       <c r="BA62" s="1"/>
       <c r="BB62" s="17"/>
@@ -5898,26 +5967,20 @@
     </row>
     <row r="63" spans="1:69">
       <c r="A63">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B63" s="3">
-        <v>24</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>37</v>
+        <v>21</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>82</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E63" s="3"/>
-      <c r="F63" s="4">
-        <f>IFERROR( HLOOKUP("BE",J63:BD$69,$A$69-$A63+1,FALSE),0)+ IFERROR( HLOOKUP("B",J63:BD$69,$A$69-$A63+1,FALSE),0)</f>
-        <v>40813</v>
-      </c>
-      <c r="G63" s="4">
-        <f>IFERROR( HLOOKUP("BE",J63:BD$69,$A$69-$A63+1,FALSE),0)+ IFERROR( HLOOKUP("E",J63:BD$69,$A$69-$A63+1,FALSE),0)</f>
-        <v>40820</v>
-      </c>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
       <c r="H63" s="4" t="s">
         <v>67</v>
       </c>
@@ -5957,30 +6020,14 @@
       <c r="AN63" s="17"/>
       <c r="AO63" s="17"/>
       <c r="AP63" s="1"/>
-      <c r="AQ63" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AR63" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AS63" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AT63" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AU63" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="AV63" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="AW63" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AX63" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="AQ63" s="1"/>
+      <c r="AR63" s="1"/>
+      <c r="AS63" s="1"/>
+      <c r="AT63" s="1"/>
+      <c r="AU63" s="17"/>
+      <c r="AV63" s="17"/>
+      <c r="AW63" s="1"/>
+      <c r="AX63" s="1"/>
       <c r="AY63" s="1"/>
       <c r="AZ63" s="1"/>
       <c r="BA63" s="1"/>
@@ -6003,26 +6050,20 @@
     </row>
     <row r="64" spans="1:69">
       <c r="A64">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B64" s="3">
-        <v>25</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>38</v>
+        <v>22</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E64" s="3"/>
-      <c r="F64" s="4">
-        <f>IFERROR( HLOOKUP("BE",J64:BD$69,$A$69-$A64+1,FALSE),0)+ IFERROR( HLOOKUP("B",J64:BD$69,$A$69-$A64+1,FALSE),0)</f>
-        <v>40821</v>
-      </c>
-      <c r="G64" s="4">
-        <f>IFERROR( HLOOKUP("BE",J64:BD$69,$A$69-$A64+1,FALSE),0)+ IFERROR( HLOOKUP("E",J64:BD$69,$A$69-$A64+1,FALSE),0)</f>
-        <v>0</v>
-      </c>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
       <c r="H64" s="4" t="s">
         <v>67</v>
       </c>
@@ -6070,27 +6111,13 @@
       <c r="AV64" s="17"/>
       <c r="AW64" s="1"/>
       <c r="AX64" s="1"/>
-      <c r="AY64" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="AZ64" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="BA64" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="BB64" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="BC64" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="BD64" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="BE64" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="AY64" s="1"/>
+      <c r="AZ64" s="1"/>
+      <c r="BA64" s="1"/>
+      <c r="BB64" s="17"/>
+      <c r="BC64" s="17"/>
+      <c r="BD64" s="1"/>
+      <c r="BE64" s="1"/>
       <c r="BF64" s="1"/>
       <c r="BG64" s="1"/>
       <c r="BH64" s="1"/>
@@ -6104,26 +6131,34 @@
       <c r="BP64" s="17"/>
       <c r="BQ64" s="17"/>
     </row>
-    <row r="65" spans="1:69" ht="18.75" customHeight="1">
+    <row r="65" spans="1:69">
       <c r="A65">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B65" s="3">
-        <v>26</v>
-      </c>
-      <c r="C65" s="27"/>
-      <c r="D65" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="C65" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="E65" s="3"/>
       <c r="F65" s="4">
-        <f>IFERROR( HLOOKUP("BE",J65:BD$69,$A$69-$A65+1,FALSE),0)+ IFERROR( HLOOKUP("B",J65:BD$69,$A$69-$A65+1,FALSE),0)</f>
-        <v>0</v>
+        <f>IFERROR( HLOOKUP("BE",J65:BD$72,$A$72-$A65+1,FALSE),0)+ IFERROR( HLOOKUP("B",J65:BD$72,$A$72-$A65+1,FALSE),0)</f>
+        <v>40821</v>
       </c>
       <c r="G65" s="4">
-        <f>IFERROR( HLOOKUP("BE",J65:BD$69,$A$69-$A65+1,FALSE),0)+ IFERROR( HLOOKUP("E",J65:BD$69,$A$69-$A65+1,FALSE),0)</f>
-        <v>0</v>
-      </c>
-      <c r="H65" s="4"/>
-      <c r="I65" s="3"/>
+        <f>IFERROR( HLOOKUP("BE",J65:BD$72,$A$72-$A65+1,FALSE),0)+ IFERROR( HLOOKUP("E",J65:BD$72,$A$72-$A65+1,FALSE),0)</f>
+        <v>40821</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="17"/>
@@ -6165,7 +6200,9 @@
       <c r="AV65" s="17"/>
       <c r="AW65" s="1"/>
       <c r="AX65" s="1"/>
-      <c r="AY65" s="1"/>
+      <c r="AY65" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="AZ65" s="1"/>
       <c r="BA65" s="1"/>
       <c r="BB65" s="17"/>
@@ -6187,224 +6224,513 @@
     </row>
     <row r="66" spans="1:69">
       <c r="A66">
-        <v>41</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B66" s="3">
+        <v>24</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" s="3"/>
+      <c r="F66" s="4">
+        <f>IFERROR( HLOOKUP("BE",J66:BD$72,$A$72-$A66+1,FALSE),0)+ IFERROR( HLOOKUP("B",J66:BD$72,$A$72-$A66+1,FALSE),0)</f>
+        <v>40813</v>
+      </c>
+      <c r="G66" s="4">
+        <f>IFERROR( HLOOKUP("BE",J66:BD$72,$A$72-$A66+1,FALSE),0)+ IFERROR( HLOOKUP("E",J66:BD$72,$A$72-$A66+1,FALSE),0)</f>
+        <v>40820</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="17"/>
+      <c r="M66" s="17"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="17"/>
+      <c r="S66" s="17"/>
+      <c r="T66" s="17"/>
+      <c r="U66" s="1"/>
+      <c r="V66" s="1"/>
+      <c r="W66" s="1"/>
+      <c r="X66" s="1"/>
+      <c r="Y66" s="1"/>
+      <c r="Z66" s="17"/>
+      <c r="AA66" s="17"/>
+      <c r="AB66" s="1"/>
+      <c r="AC66" s="1"/>
+      <c r="AD66" s="1"/>
+      <c r="AE66" s="1"/>
+      <c r="AF66" s="1"/>
+      <c r="AG66" s="17"/>
+      <c r="AH66" s="17"/>
+      <c r="AI66" s="1"/>
+      <c r="AJ66" s="1"/>
+      <c r="AK66" s="1"/>
+      <c r="AL66" s="1"/>
+      <c r="AM66" s="1"/>
+      <c r="AN66" s="17"/>
+      <c r="AO66" s="17"/>
+      <c r="AP66" s="1"/>
+      <c r="AQ66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AR66" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS66" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT66" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU66" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV66" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AW66" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AY66" s="1"/>
+      <c r="AZ66" s="1"/>
+      <c r="BA66" s="1"/>
+      <c r="BB66" s="17"/>
+      <c r="BC66" s="17"/>
+      <c r="BD66" s="1"/>
+      <c r="BE66" s="1"/>
+      <c r="BF66" s="1"/>
+      <c r="BG66" s="1"/>
+      <c r="BH66" s="1"/>
+      <c r="BI66" s="17"/>
+      <c r="BJ66" s="17"/>
+      <c r="BK66" s="1"/>
+      <c r="BL66" s="1"/>
+      <c r="BM66" s="1"/>
+      <c r="BN66" s="1"/>
+      <c r="BO66" s="1"/>
+      <c r="BP66" s="17"/>
+      <c r="BQ66" s="17"/>
     </row>
     <row r="67" spans="1:69">
       <c r="A67">
+        <v>39</v>
+      </c>
+      <c r="B67" s="3">
+        <v>25</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" s="3"/>
+      <c r="F67" s="4">
+        <f>IFERROR( HLOOKUP("BE",J67:BD$72,$A$72-$A67+1,FALSE),0)+ IFERROR( HLOOKUP("B",J67:BD$72,$A$72-$A67+1,FALSE),0)</f>
+        <v>40821</v>
+      </c>
+      <c r="G67" s="4">
+        <f>IFERROR( HLOOKUP("BE",J67:BD$72,$A$72-$A67+1,FALSE),0)+ IFERROR( HLOOKUP("E",J67:BD$72,$A$72-$A67+1,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="17"/>
+      <c r="M67" s="17"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="17"/>
+      <c r="S67" s="17"/>
+      <c r="T67" s="17"/>
+      <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
+      <c r="W67" s="1"/>
+      <c r="X67" s="1"/>
+      <c r="Y67" s="1"/>
+      <c r="Z67" s="17"/>
+      <c r="AA67" s="17"/>
+      <c r="AB67" s="1"/>
+      <c r="AC67" s="1"/>
+      <c r="AD67" s="1"/>
+      <c r="AE67" s="1"/>
+      <c r="AF67" s="1"/>
+      <c r="AG67" s="17"/>
+      <c r="AH67" s="17"/>
+      <c r="AI67" s="1"/>
+      <c r="AJ67" s="1"/>
+      <c r="AK67" s="1"/>
+      <c r="AL67" s="1"/>
+      <c r="AM67" s="1"/>
+      <c r="AN67" s="17"/>
+      <c r="AO67" s="17"/>
+      <c r="AP67" s="1"/>
+      <c r="AQ67" s="1"/>
+      <c r="AR67" s="1"/>
+      <c r="AS67" s="1"/>
+      <c r="AT67" s="1"/>
+      <c r="AU67" s="17"/>
+      <c r="AV67" s="17"/>
+      <c r="AW67" s="1"/>
+      <c r="AX67" s="1"/>
+      <c r="AY67" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="AZ67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BA67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB67" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="BC67" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="BD67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BE67" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BF67" s="1"/>
+      <c r="BG67" s="1"/>
+      <c r="BH67" s="1"/>
+      <c r="BI67" s="17"/>
+      <c r="BJ67" s="17"/>
+      <c r="BK67" s="1"/>
+      <c r="BL67" s="1"/>
+      <c r="BM67" s="1"/>
+      <c r="BN67" s="1"/>
+      <c r="BO67" s="1"/>
+      <c r="BP67" s="17"/>
+      <c r="BQ67" s="17"/>
+    </row>
+    <row r="68" spans="1:69" ht="18.75" customHeight="1">
+      <c r="A68">
+        <v>40</v>
+      </c>
+      <c r="B68" s="3">
+        <v>26</v>
+      </c>
+      <c r="C68" s="27"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="4">
+        <f>IFERROR( HLOOKUP("BE",J68:BD$72,$A$72-$A68+1,FALSE),0)+ IFERROR( HLOOKUP("B",J68:BD$72,$A$72-$A68+1,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G68" s="4">
+        <f>IFERROR( HLOOKUP("BE",J68:BD$72,$A$72-$A68+1,FALSE),0)+ IFERROR( HLOOKUP("E",J68:BD$72,$A$72-$A68+1,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H68" s="4"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="17"/>
+      <c r="M68" s="17"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="17"/>
+      <c r="S68" s="17"/>
+      <c r="T68" s="17"/>
+      <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
+      <c r="W68" s="1"/>
+      <c r="X68" s="1"/>
+      <c r="Y68" s="1"/>
+      <c r="Z68" s="17"/>
+      <c r="AA68" s="17"/>
+      <c r="AB68" s="1"/>
+      <c r="AC68" s="1"/>
+      <c r="AD68" s="1"/>
+      <c r="AE68" s="1"/>
+      <c r="AF68" s="1"/>
+      <c r="AG68" s="17"/>
+      <c r="AH68" s="17"/>
+      <c r="AI68" s="1"/>
+      <c r="AJ68" s="1"/>
+      <c r="AK68" s="1"/>
+      <c r="AL68" s="1"/>
+      <c r="AM68" s="1"/>
+      <c r="AN68" s="17"/>
+      <c r="AO68" s="17"/>
+      <c r="AP68" s="1"/>
+      <c r="AQ68" s="1"/>
+      <c r="AR68" s="1"/>
+      <c r="AS68" s="1"/>
+      <c r="AT68" s="1"/>
+      <c r="AU68" s="17"/>
+      <c r="AV68" s="17"/>
+      <c r="AW68" s="1"/>
+      <c r="AX68" s="1"/>
+      <c r="AY68" s="1"/>
+      <c r="AZ68" s="1"/>
+      <c r="BA68" s="1"/>
+      <c r="BB68" s="17"/>
+      <c r="BC68" s="17"/>
+      <c r="BD68" s="1"/>
+      <c r="BE68" s="1"/>
+      <c r="BF68" s="1"/>
+      <c r="BG68" s="1"/>
+      <c r="BH68" s="1"/>
+      <c r="BI68" s="17"/>
+      <c r="BJ68" s="17"/>
+      <c r="BK68" s="1"/>
+      <c r="BL68" s="1"/>
+      <c r="BM68" s="1"/>
+      <c r="BN68" s="1"/>
+      <c r="BO68" s="1"/>
+      <c r="BP68" s="17"/>
+      <c r="BQ68" s="17"/>
+    </row>
+    <row r="69" spans="1:69">
+      <c r="A69">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70" spans="1:69">
+      <c r="A70">
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:69">
-      <c r="A68">
+    <row r="71" spans="1:69">
+      <c r="A71">
         <v>43</v>
       </c>
     </row>
-    <row r="69" spans="1:69" s="10" customFormat="1">
-      <c r="A69">
+    <row r="72" spans="1:69" s="10" customFormat="1">
+      <c r="A72">
         <v>44</v>
       </c>
-      <c r="C69" s="30" t="s">
+      <c r="C72" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="J69" s="5">
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="J72" s="5">
         <f>J8</f>
         <v>40780</v>
       </c>
-      <c r="K69" s="5">
-        <f t="shared" ref="K69:BD69" si="1">K8</f>
+      <c r="K72" s="5">
+        <f t="shared" ref="K72:BD72" si="1">K8</f>
         <v>40781</v>
       </c>
-      <c r="L69" s="5">
+      <c r="L72" s="5">
         <f t="shared" si="1"/>
         <v>40782</v>
       </c>
-      <c r="M69" s="5">
+      <c r="M72" s="5">
         <f t="shared" si="1"/>
         <v>40783</v>
       </c>
-      <c r="N69" s="5">
+      <c r="N72" s="5">
         <f t="shared" si="1"/>
         <v>40784</v>
       </c>
-      <c r="O69" s="5">
+      <c r="O72" s="5">
         <f t="shared" si="1"/>
         <v>40785</v>
       </c>
-      <c r="P69" s="5">
+      <c r="P72" s="5">
         <f t="shared" si="1"/>
         <v>40786</v>
       </c>
-      <c r="Q69" s="5">
+      <c r="Q72" s="5">
         <f t="shared" si="1"/>
         <v>40787</v>
       </c>
-      <c r="R69" s="5">
+      <c r="R72" s="5">
         <f t="shared" si="1"/>
         <v>40788</v>
       </c>
-      <c r="S69" s="5">
+      <c r="S72" s="5">
         <f t="shared" si="1"/>
         <v>40789</v>
       </c>
-      <c r="T69" s="5">
+      <c r="T72" s="5">
         <f t="shared" si="1"/>
         <v>40790</v>
       </c>
-      <c r="U69" s="5">
+      <c r="U72" s="5">
         <f t="shared" si="1"/>
         <v>40791</v>
       </c>
-      <c r="V69" s="5">
+      <c r="V72" s="5">
         <f t="shared" si="1"/>
         <v>40792</v>
       </c>
-      <c r="W69" s="5">
+      <c r="W72" s="5">
         <f t="shared" si="1"/>
         <v>40793</v>
       </c>
-      <c r="X69" s="5">
+      <c r="X72" s="5">
         <f t="shared" si="1"/>
         <v>40794</v>
       </c>
-      <c r="Y69" s="5">
+      <c r="Y72" s="5">
         <f t="shared" si="1"/>
         <v>40795</v>
       </c>
-      <c r="Z69" s="5">
+      <c r="Z72" s="5">
         <f t="shared" si="1"/>
         <v>40796</v>
       </c>
-      <c r="AA69" s="5">
+      <c r="AA72" s="5">
         <f t="shared" si="1"/>
         <v>40797</v>
       </c>
-      <c r="AB69" s="5">
+      <c r="AB72" s="5">
         <f t="shared" si="1"/>
         <v>40798</v>
       </c>
-      <c r="AC69" s="5">
+      <c r="AC72" s="5">
         <f t="shared" si="1"/>
         <v>40799</v>
       </c>
-      <c r="AD69" s="5">
+      <c r="AD72" s="5">
         <f t="shared" si="1"/>
         <v>40800</v>
       </c>
-      <c r="AE69" s="5">
+      <c r="AE72" s="5">
         <f t="shared" si="1"/>
         <v>40801</v>
       </c>
-      <c r="AF69" s="5">
+      <c r="AF72" s="5">
         <f t="shared" si="1"/>
         <v>40802</v>
       </c>
-      <c r="AG69" s="5">
+      <c r="AG72" s="5">
         <f t="shared" si="1"/>
         <v>40803</v>
       </c>
-      <c r="AH69" s="5">
+      <c r="AH72" s="5">
         <f t="shared" si="1"/>
         <v>40804</v>
       </c>
-      <c r="AI69" s="5">
+      <c r="AI72" s="5">
         <f t="shared" si="1"/>
         <v>40805</v>
       </c>
-      <c r="AJ69" s="5">
+      <c r="AJ72" s="5">
         <f t="shared" si="1"/>
         <v>40806</v>
       </c>
-      <c r="AK69" s="5">
+      <c r="AK72" s="5">
         <f t="shared" si="1"/>
         <v>40807</v>
       </c>
-      <c r="AL69" s="5">
+      <c r="AL72" s="5">
         <f t="shared" si="1"/>
         <v>40808</v>
       </c>
-      <c r="AM69" s="5">
+      <c r="AM72" s="5">
         <f t="shared" si="1"/>
         <v>40809</v>
       </c>
-      <c r="AN69" s="5">
+      <c r="AN72" s="5">
         <f t="shared" si="1"/>
         <v>40810</v>
       </c>
-      <c r="AO69" s="5">
+      <c r="AO72" s="5">
         <f t="shared" si="1"/>
         <v>40811</v>
       </c>
-      <c r="AP69" s="5">
+      <c r="AP72" s="5">
         <f t="shared" si="1"/>
         <v>40812</v>
       </c>
-      <c r="AQ69" s="5">
+      <c r="AQ72" s="5">
         <f t="shared" si="1"/>
         <v>40813</v>
       </c>
-      <c r="AR69" s="5">
+      <c r="AR72" s="5">
         <f t="shared" si="1"/>
         <v>40814</v>
       </c>
-      <c r="AS69" s="5">
+      <c r="AS72" s="5">
         <f t="shared" si="1"/>
         <v>40815</v>
       </c>
-      <c r="AT69" s="5">
+      <c r="AT72" s="5">
         <f t="shared" si="1"/>
         <v>40816</v>
       </c>
-      <c r="AU69" s="5">
+      <c r="AU72" s="5">
         <f t="shared" si="1"/>
         <v>40817</v>
       </c>
-      <c r="AV69" s="5">
+      <c r="AV72" s="5">
         <f t="shared" si="1"/>
         <v>40818</v>
       </c>
-      <c r="AW69" s="5">
+      <c r="AW72" s="5">
         <f t="shared" si="1"/>
         <v>40819</v>
       </c>
-      <c r="AX69" s="5">
+      <c r="AX72" s="5">
         <f t="shared" si="1"/>
         <v>40820</v>
       </c>
-      <c r="AY69" s="5">
+      <c r="AY72" s="5">
         <f t="shared" si="1"/>
         <v>40821</v>
       </c>
-      <c r="AZ69" s="5">
+      <c r="AZ72" s="5">
         <f t="shared" si="1"/>
         <v>40822</v>
       </c>
-      <c r="BA69" s="5">
+      <c r="BA72" s="5">
         <f t="shared" si="1"/>
         <v>40823</v>
       </c>
-      <c r="BB69" s="5">
+      <c r="BB72" s="5">
         <f t="shared" si="1"/>
         <v>40824</v>
       </c>
-      <c r="BC69" s="5">
+      <c r="BC72" s="5">
         <f t="shared" si="1"/>
         <v>40825</v>
       </c>
-      <c r="BD69" s="5">
+      <c r="BD72" s="5">
         <f t="shared" si="1"/>
         <v>40826</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A8:BQ69"/>
+  <autoFilter ref="A8:BQ72"/>
   <mergeCells count="1">
     <mergeCell ref="K2:Q2"/>
   </mergeCells>
-  <conditionalFormatting sqref="J66:AW66 J13:BD13 J10:AF11 AG11 AH10:BD11 J15:BD22 J24:BD65 AU11:AV65 BB11:BC65 BE10:BQ65">
+  <conditionalFormatting sqref="J69:AW69 J44:BQ68 J13:BD13 J10:AF11 AG11 AH10:BD11 J15:BD22 AU11:AV38 BB11:BC38 J24:BD43 BE10:BQ43">
     <cfRule type="cellIs" dxfId="6" priority="34" operator="equal">
       <formula>"-"</formula>
     </cfRule>
@@ -6415,12 +6741,12 @@
       <formula>"B"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J13:BD13 J10:AF11 AG11 AH10:BD11 J15:BD22 J24:BD65 AU11:AV65 BB11:BC65 BE10:BQ65">
+  <conditionalFormatting sqref="J44:BQ68 J13:BD13 J10:AF11 AG11 AH10:BD11 J15:BD22 AU11:AV38 BB11:BC38 J24:BD43 BE10:BQ43">
     <cfRule type="cellIs" dxfId="3" priority="33" operator="equal">
       <formula>"BE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10:H11 H13 H15:H22 H24:H65">
+  <conditionalFormatting sqref="H10:H11 H13 H15:H22 H24:H68">
     <cfRule type="cellIs" dxfId="2" priority="15" operator="equal">
       <formula>$E$4</formula>
     </cfRule>
@@ -6428,16 +6754,16 @@
       <formula>AND(H10&lt;&gt;$E$4,$G$10&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11 H13 H15:H22 H24:H65">
+  <conditionalFormatting sqref="H11 H13 H15:H22 H24:H68">
     <cfRule type="expression" dxfId="0" priority="19">
       <formula>AND(H11&lt;&gt;$E$4,$G$10&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H65">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H68">
       <formula1>$E$2:$E$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D11 D13 D15:D22 D24:D65">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13 D15:D22 D24:D68 D10:D11">
       <formula1>$C$2:$C$4</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>